<commit_message>
data loader code added - changes to strcut fields
</commit_message>
<xml_diff>
--- a/cases/SMIB_Chow/SMIB_RL_Line_DrCui.xlsx
+++ b/cases/SMIB_Chow/SMIB_RL_Line_DrCui.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\aaliqureshi\andes\andes\cases\SMIB_Chow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aali27/Work/repos/emt_simulator_basic/cases/SMIB_Chow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0207B6-C9EE-491D-A64C-0450EC03BFE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DFCDD9-1249-CA4B-A4DF-3CF8809DA141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25740" yWindow="3435" windowWidth="18435" windowHeight="9735" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="84">
   <si>
     <t>field</t>
   </si>
@@ -130,9 +130,6 @@
     <t>q0</t>
   </si>
   <si>
-    <t>PQ_1</t>
-  </si>
-  <si>
     <t>PQ 1</t>
   </si>
   <si>
@@ -229,12 +226,6 @@
     <t>rate_c</t>
   </si>
   <si>
-    <t>Line_1</t>
-  </si>
-  <si>
-    <t>Line_2</t>
-  </si>
-  <si>
     <t>Line 1</t>
   </si>
   <si>
@@ -281,12 +272,6 @@
   </si>
   <si>
     <t>gammaq</t>
-  </si>
-  <si>
-    <t>GENCLS_1</t>
-  </si>
-  <si>
-    <t>GENCLS_2</t>
   </si>
   <si>
     <t>GENCLS 1</t>
@@ -670,9 +655,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -692,7 +677,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -703,7 +688,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -714,7 +699,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -734,14 +719,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -758,22 +743,22 @@
         <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -784,7 +769,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -813,12 +798,12 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -847,12 +832,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>20</v>
+      <c r="B2">
+        <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -890,9 +875,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -936,7 +921,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -980,7 +965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1024,7 +1009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1079,12 +1064,12 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1119,18 +1104,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>33</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -1165,12 +1150,12 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1184,7 +1169,7 @@
         <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>21</v>
@@ -1193,7 +1178,7 @@
         <v>15</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>31</v>
@@ -1202,16 +1187,16 @@
         <v>32</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>24</v>
@@ -1223,24 +1208,24 @@
         <v>23</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>43</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>44</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -1296,12 +1281,12 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1315,7 +1300,7 @@
         <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>21</v>
@@ -1324,7 +1309,7 @@
         <v>15</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>31</v>
@@ -1333,16 +1318,16 @@
         <v>32</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>24</v>
@@ -1354,27 +1339,27 @@
         <v>23</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>45</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>46</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -1433,12 +1418,12 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1452,64 +1437,64 @@
         <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>30</v>
@@ -1521,18 +1506,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>66</v>
+      <c r="B2">
+        <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1595,18 +1580,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>67</v>
+      <c r="B3">
+        <v>2</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1683,9 +1668,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1699,7 +1684,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1710,7 +1695,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1722,14 +1707,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1746,75 +1731,75 @@
         <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="T1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>81</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>86</v>
-      </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I2">
         <v>100</v>
@@ -1859,24 +1844,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>85</v>
+      <c r="B3">
+        <v>2</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I3">
         <v>1000000000</v>

</xml_diff>